<commit_message>
added company info component
</commit_message>
<xml_diff>
--- a/src/assets/Data/PDF Builder.xlsx
+++ b/src/assets/Data/PDF Builder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Raksha\Projects\Javascript Projects\Equipment Installation diagram app\MountingDiagram app\src\assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6FCE93-4C3A-4A1D-AF08-F0AC0E1B3DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E03EE2-058C-4ECA-BEA6-5E52E0DF5A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42170" yWindow="-1550" windowWidth="12140" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42170" yWindow="-1550" windowWidth="12140" windowHeight="8880" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Screen MFR" sheetId="1" r:id="rId1"/>
@@ -232,9 +232,6 @@
     <t>Brand</t>
   </si>
   <si>
-    <t>Maximum Load (lbs)</t>
-  </si>
-  <si>
     <t>VESA's</t>
   </si>
   <si>
@@ -311,6 +308,9 @@
   </si>
   <si>
     <t>Screen</t>
+  </si>
+  <si>
+    <t>MaximumLoad</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,7 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -610,7 +610,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1704,7 +1704,9 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -1723,36 +1725,36 @@
         <v>68</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="C2" s="5">
         <v>200</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E2" s="5">
         <v>27.41</v>
@@ -1769,16 +1771,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="5">
         <v>300</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="5">
         <v>45</v>
@@ -1795,16 +1797,16 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="5">
         <v>200</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="5">
         <v>27.37</v>
@@ -1821,16 +1823,16 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="5">
         <v>200</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="5">
         <v>34.5</v>
@@ -1847,10 +1849,10 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="C6" s="5">
         <v>250</v>
@@ -1871,16 +1873,16 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="C7" s="5">
         <v>200</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E7" s="5">
         <v>28.84</v>
@@ -1897,16 +1899,16 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="5">
         <v>250</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E8" s="5">
         <v>34.75</v>
@@ -1923,10 +1925,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="5">
         <v>350</v>
@@ -1947,10 +1949,10 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="3">
         <v>350</v>
@@ -2006,10 +2008,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="C2" s="1">
         <v>6.25</v>

</xml_diff>